<commit_message>
Added Calculations for Stock only. Not fund
</commit_message>
<xml_diff>
--- a/BotConfig.xlsx
+++ b/BotConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Prj-ABC\robot\ABCFundRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC069B5E-ADB5-46F2-AEA9-B55CCD5F7405}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB657E-2EAB-4603-AF89-D7466D6C101A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="510" windowWidth="18015" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="11064" windowHeight="10152" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="2" r:id="rId1"/>
@@ -786,17 +786,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8194B291-89E1-4C17-A6E2-A7ADC84E2330}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -804,7 +804,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -812,7 +812,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -820,7 +820,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -828,7 +828,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -836,7 +836,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -844,7 +844,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -852,7 +852,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -860,32 +860,32 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>142</v>
       </c>
@@ -902,22 +902,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -937,7 +937,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -957,7 +957,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -977,7 +977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -997,7 +997,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Change sql into Azure
</commit_message>
<xml_diff>
--- a/BotConfig.xlsx
+++ b/BotConfig.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Prj-ABC\robot\ABCFundRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B827ECC7-6319-4CBF-A14F-F24A7A9D69CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC82EB-3C06-4436-BF1C-EC976E0764D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="876" yWindow="0" windowWidth="21912" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6600" yWindow="0" windowWidth="16356" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="2" r:id="rId1"/>
     <sheet name="Stock" sheetId="1" r:id="rId2"/>
     <sheet name="Periodic" sheetId="3" r:id="rId3"/>
-    <sheet name="Fund" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="146">
   <si>
     <t>https://finance.yahoo.com/quote/%255ESTI%253FP%253D%255ESTI/history/</t>
   </si>
@@ -258,21 +257,6 @@
     <t>sqlConnectionString</t>
   </si>
   <si>
-    <t>Server=tcp:ust.database.windows.net,1433;Initial Catalog=abcfunddb;Persist Security Info=False;User ID=;Password=;MultipleActiveResultSets=False;Encrypt=True;TrustServerCertificate=False;Connection Timeout=30;</t>
-  </si>
-  <si>
-    <t>sqlUsername</t>
-  </si>
-  <si>
-    <t>sqlPassword</t>
-  </si>
-  <si>
-    <t>jsazure</t>
-  </si>
-  <si>
-    <t>USTpass@999</t>
-  </si>
-  <si>
     <t>CsvPath</t>
   </si>
   <si>
@@ -462,31 +446,35 @@
     <t>Server=DESKTOP-483N209\SQLEXPRESS;Database=abcdb;persist security info=True;Integrated Security=SSPI;</t>
   </si>
   <si>
-    <t>tempAzureConnectionString</t>
-  </si>
-  <si>
     <t>providerName</t>
   </si>
   <si>
     <t>System.Data.SqlClient</t>
+  </si>
+  <si>
+    <t>sqlCredentials</t>
+  </si>
+  <si>
+    <t>sql_azure_credential</t>
+  </si>
+  <si>
+    <t>azureConnectionString</t>
+  </si>
+  <si>
+    <t>orchestratorFilePath</t>
+  </si>
+  <si>
+    <t>https://cloud.uipath.com/ustglobalsingap/USTGlobalSingaporeDefault/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,17 +497,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -801,7 +786,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,108 +808,106 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>144</v>
       </c>
-      <c r="B4" t="s">
-        <v>76</v>
+      <c r="B4" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
+        <v>141</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>136</v>
+      <c r="B12" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{4437148C-DDA2-4765-B700-3EEDCCFD1D0A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -961,10 +944,10 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -981,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1001,10 +984,10 @@
         <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1021,10 +1004,10 @@
         <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1041,10 +1024,10 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1061,10 +1044,10 @@
         <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,10 +1064,10 @@
         <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1101,10 +1084,10 @@
         <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1121,10 +1104,10 @@
         <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1141,10 +1124,10 @@
         <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1161,10 +1144,10 @@
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1181,10 +1164,10 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1221,10 +1204,10 @@
         <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1241,10 +1224,10 @@
         <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1261,10 +1244,10 @@
         <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1281,10 +1264,10 @@
         <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1301,10 +1284,10 @@
         <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1321,10 +1304,10 @@
         <v>72</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1341,10 +1324,10 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1361,10 +1344,10 @@
         <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,10 +1364,10 @@
         <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1401,10 +1384,10 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1421,10 +1404,10 @@
         <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1489,30 +1472,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794D1982-139D-4190-9E98-D4356E735F47}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>